<commit_message>
Test pasando en verde.
rama Modulo1Tania todos los tests pasando.
He añadido las anotaciones al modelo, corregido en RList el load para que acepte celdas en blanco. También he corregido algun error de formato y he formateado algunas clases. Corregido algunos tests para adaptarse a los nuevos requisitos. Refactorización de la query findByDni por findByIdentificator.
</commit_message>
<xml_diff>
--- a/src/test/resources/test2.xlsx
+++ b/src/test/resources/test2.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\ASW\Loader_e5a\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2025" yWindow="1545" windowWidth="12735" windowHeight="4515"/>
+    <workbookView xWindow="2025" yWindow="1545" windowWidth="12735" windowHeight="4515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -67,17 +71,17 @@
     <t>ST1Oviedo</t>
   </si>
   <si>
-    <t>43,24&amp;-5,78</t>
-  </si>
-  <si>
-    <t>43,36&amp;-5,85</t>
+    <t>43.36&amp;-5.85</t>
+  </si>
+  <si>
+    <t>43.24&amp;-5.78</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +93,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -115,11 +127,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -393,18 +406,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,7 +464,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>4</v>
@@ -468,7 +481,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>11</v>
@@ -480,12 +493,15 @@
         <v>2</v>
       </c>
       <c r="G4" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId4"/>

</xml_diff>

<commit_message>
Ahora se comprueba que el sensor tenga Localizacion obligatoriamente
</commit_message>
<xml_diff>
--- a/src/test/resources/test2.xlsx
+++ b/src/test/resources/test2.xlsx
@@ -1,26 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\ASW\Loader_e5a\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/IsmaCadenas/git/Loader_e5a/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2025" yWindow="1545" windowWidth="12735" windowHeight="4515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11100" yWindow="8400" windowWidth="14500" windowHeight="6380"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -71,16 +74,16 @@
     <t>ST1Oviedo</t>
   </si>
   <si>
+    <t>43.24&amp;-5.78</t>
+  </si>
+  <si>
     <t>43.36&amp;-5.85</t>
-  </si>
-  <si>
-    <t>43.24&amp;-5.78</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -413,22 +416,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="35.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="1" max="2" width="23.5" customWidth="1"/>
+    <col min="3" max="3" width="35.5" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,7 +448,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -459,12 +462,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>4</v>
@@ -476,12 +479,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>11</v>
@@ -494,14 +497,14 @@
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C7" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId4"/>

</xml_diff>